<commit_message>
updated classes + screenshots
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsote\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsote\Desktop\sfmproject\SFMproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70523043-AADF-425E-A0A2-52E8B5745E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05139265-45AF-4013-9A9D-1E7B8B83A3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FDAA1B2B-9794-4B2D-A776-BFD1CFC738AA}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FDAA1B2B-9794-4B2D-A776-BFD1CFC738AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -640,26 +640,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C5D562-07E2-4356-AAE1-0AB7DC2E2767}">
   <dimension ref="B1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
-    <col min="11" max="11" width="22.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
@@ -675,7 +675,7 @@
       <c r="K2" s="17"/>
       <c r="L2" s="18"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
@@ -707,7 +707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -737,7 +737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -767,7 +767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -797,7 +797,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>4</v>
       </c>
@@ -827,15 +827,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H9" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H10" s="9" t="s">
         <v>11</v>
       </c>
@@ -843,7 +843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H11" s="2">
         <v>1</v>
       </c>
@@ -851,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H12" s="2">
         <v>1</v>
       </c>
@@ -859,7 +859,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H13" s="2">
         <v>1</v>
       </c>
@@ -867,7 +867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H14" s="2">
         <v>2</v>
       </c>
@@ -875,7 +875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H15" s="2">
         <v>2</v>
       </c>
@@ -883,7 +883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="H16" s="2">
         <v>3</v>
       </c>
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H17" s="2">
         <v>3</v>
       </c>
@@ -899,7 +899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="2">
         <v>3</v>
       </c>
@@ -907,7 +907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="8:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H19" s="5">
         <v>4</v>
       </c>
@@ -928,15 +928,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentum" ma:contentTypeID="0x0101000D0EEFF6460821469BAE130745D7B155" ma:contentTypeVersion="4" ma:contentTypeDescription="Új dokumentum létrehozása." ma:contentTypeScope="" ma:versionID="867c82898aacd3f9e69f4bc9ca9b936b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f9be07df-78c1-48a7-b0fc-c55a6006306c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="83fb249aa58dc3e6b135f165d0f07e5e" ns3:_="">
     <xsd:import namespace="f9be07df-78c1-48a7-b0fc-c55a6006306c"/>
@@ -1082,6 +1073,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1089,14 +1089,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A85B9D47-1982-4715-9A85-195DB072E10F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E32EE3D4-2415-4464-AED3-AD3392F7C1E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1110,6 +1102,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A85B9D47-1982-4715-9A85-195DB072E10F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>